<commit_message>
updated BOM, was missing a few things
</commit_message>
<xml_diff>
--- a/v1/BOM/gateway_shield_bom.xlsx
+++ b/v1/BOM/gateway_shield_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Description</t>
   </si>
@@ -60,15 +60,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>0.1" 12-pin header</t>
-  </si>
-  <si>
-    <t>68000-412HLF</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>2Mb SPI Flash</t>
   </si>
   <si>
-    <t>SST25VF020-20-4I-SAE</t>
-  </si>
-  <si>
     <t>20ppm, 9pF, 32.768KHz crystal</t>
   </si>
   <si>
@@ -165,9 +153,6 @@
     <t>R1, R2</t>
   </si>
   <si>
-    <t>JP3</t>
-  </si>
-  <si>
     <t>0.05" 10-pin header</t>
   </si>
   <si>
@@ -178,19 +163,63 @@
   </si>
   <si>
     <t>20021121-00010C4LF</t>
+  </si>
+  <si>
+    <t>2Mb</t>
+  </si>
+  <si>
+    <t>Microcip</t>
+  </si>
+  <si>
+    <t>SST25VF020B-80-4I-SAE</t>
+  </si>
+  <si>
+    <t>3.5mmx2.9mm Tactile Switch</t>
+  </si>
+  <si>
+    <t>EVP-AA202K</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>0.1" 12-pin female header</t>
+  </si>
+  <si>
+    <t>PPTC121LFBN-RC</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>Micro USB Type B Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,6 +260,19 @@
       <color theme="10"/>
       <name val="Museo 700"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Museo 700"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,7 +291,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -268,8 +310,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,8 +323,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -297,6 +346,8 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -627,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -645,15 +696,15 @@
     <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -662,273 +713,346 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:14" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" s="5"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" customFormat="1">
       <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="B7" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="H10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2" t="s">
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H11" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H8" r:id="rId5"/>
-    <hyperlink ref="H6" r:id="rId6"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H9" r:id="rId4"/>
+    <hyperlink ref="H7" r:id="rId5"/>
+    <hyperlink ref="H11" r:id="rId6"/>
     <hyperlink ref="H10" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
-    <hyperlink ref="H11" r:id="rId9"/>
-    <hyperlink ref="H7" r:id="rId10"/>
-    <hyperlink ref="H12" r:id="rId11"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H12" r:id="rId9"/>
+    <hyperlink ref="H4" r:id="rId10"/>
+    <hyperlink ref="H14" r:id="rId11"/>
+    <hyperlink ref="H5" r:id="rId12"/>
+    <hyperlink ref="H13" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>